<commit_message>
Use Postgres for wakeups
</commit_message>
<xml_diff>
--- a/quiz_database.xlsx
+++ b/quiz_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\OneDrive\ドキュメント\趣味\SHIFT\asakatsu_light\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774998A7-7AAE-44F6-AED0-2EC3B1E49309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B126D575-C5BA-4581-974E-B7A3B60A3280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="559">
   <si>
     <t>id</t>
   </si>
@@ -630,6 +630,1074 @@
   </si>
   <si>
     <t>公開鍵と秘密鍵</t>
+  </si>
+  <si>
+    <t>2進数 (1111)₂ を10進数で表したものはどれ？</t>
+  </si>
+  <si>
+    <t>1111₂ = 8+4+2+1 = 15</t>
+  </si>
+  <si>
+    <t>10進数 7 を2進数で表したものはどれ？</t>
+  </si>
+  <si>
+    <t>7 = 111₂</t>
+  </si>
+  <si>
+    <t>コンピュータで扱われる文字コードの例はどれ？</t>
+  </si>
+  <si>
+    <t>ASCII</t>
+  </si>
+  <si>
+    <t>HTTP</t>
+  </si>
+  <si>
+    <t>TCP</t>
+  </si>
+  <si>
+    <t>ASCIIは文字コード</t>
+  </si>
+  <si>
+    <t>ソフトウェアのバージョン管理に使われるツールはどれ？</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>PowerPoint</t>
+  </si>
+  <si>
+    <t>FTP</t>
+  </si>
+  <si>
+    <t>Gitはバージョン管理</t>
+  </si>
+  <si>
+    <t>OSのスケジューリングが対象とするものは？</t>
+  </si>
+  <si>
+    <t>電源</t>
+  </si>
+  <si>
+    <t>プロセス</t>
+  </si>
+  <si>
+    <t>記憶装置</t>
+  </si>
+  <si>
+    <t>ネットワーク</t>
+  </si>
+  <si>
+    <t>CPU割当を管理</t>
+  </si>
+  <si>
+    <t>CPUが直接実行できる命令は何で書かれている？</t>
+  </si>
+  <si>
+    <t>高級言語</t>
+  </si>
+  <si>
+    <t>機械語</t>
+  </si>
+  <si>
+    <t>CPUは機械語を実行</t>
+  </si>
+  <si>
+    <t>SSDの特徴として正しいものはどれ？</t>
+  </si>
+  <si>
+    <t>磁気で記録</t>
+  </si>
+  <si>
+    <t>可動部がある</t>
+  </si>
+  <si>
+    <t>高速アクセス</t>
+  </si>
+  <si>
+    <t>揮発性</t>
+  </si>
+  <si>
+    <t>SSDは高速</t>
+  </si>
+  <si>
+    <t>HDDと比べたSSDの利点はどれ？</t>
+  </si>
+  <si>
+    <t>容量が必ず大きい</t>
+  </si>
+  <si>
+    <t>価格が安い</t>
+  </si>
+  <si>
+    <t>耐衝撃性が高い</t>
+  </si>
+  <si>
+    <t>書き換え不可</t>
+  </si>
+  <si>
+    <t>SSDは衝撃に強い</t>
+  </si>
+  <si>
+    <t>IPアドレスのIPv4は何ビットか？</t>
+  </si>
+  <si>
+    <t>IPv4は32bit</t>
+  </si>
+  <si>
+    <t>IPv6アドレスの特徴はどれ？</t>
+  </si>
+  <si>
+    <t>表記が10進数</t>
+  </si>
+  <si>
+    <t>アドレス空間が広い</t>
+  </si>
+  <si>
+    <t>非公開のみ</t>
+  </si>
+  <si>
+    <t>IPv6は128bit</t>
+  </si>
+  <si>
+    <t>TCPの特徴として正しいものはどれ？</t>
+  </si>
+  <si>
+    <t>信頼性が低い</t>
+  </si>
+  <si>
+    <t>コネクション型</t>
+  </si>
+  <si>
+    <t>高速だが不安定</t>
+  </si>
+  <si>
+    <t>暗号化必須</t>
+  </si>
+  <si>
+    <t>TCPは信頼性あり</t>
+  </si>
+  <si>
+    <t>UDPの特徴として正しいものはどれ？</t>
+  </si>
+  <si>
+    <t>必ず再送する</t>
+  </si>
+  <si>
+    <t>信頼性が高い</t>
+  </si>
+  <si>
+    <t>コネクションレス</t>
+  </si>
+  <si>
+    <t>暗号化される</t>
+  </si>
+  <si>
+    <t>UDPはコネクションレス</t>
+  </si>
+  <si>
+    <t>ネットワークで用いられるポート番号の役割は？</t>
+  </si>
+  <si>
+    <t>機器識別</t>
+  </si>
+  <si>
+    <t>通信相手識別</t>
+  </si>
+  <si>
+    <t>アプリケーション識別</t>
+  </si>
+  <si>
+    <t>暗号化</t>
+  </si>
+  <si>
+    <t>ポートはアプリ識別</t>
+  </si>
+  <si>
+    <t>HTTPのデフォルトポート番号は？</t>
+  </si>
+  <si>
+    <t>HTTPは80</t>
+  </si>
+  <si>
+    <t>HTTPSのデフォルトポート番号は？</t>
+  </si>
+  <si>
+    <t>HTTPSは443</t>
+  </si>
+  <si>
+    <t>SQLで条件を指定する句はどれ？</t>
+  </si>
+  <si>
+    <t>WHERE</t>
+  </si>
+  <si>
+    <t>ORDER</t>
+  </si>
+  <si>
+    <t>GROUP</t>
+  </si>
+  <si>
+    <t>LIMIT</t>
+  </si>
+  <si>
+    <t>WHERE句</t>
+  </si>
+  <si>
+    <t>SQLで並び替えを行う句はどれ？</t>
+  </si>
+  <si>
+    <t>GROUP BY</t>
+  </si>
+  <si>
+    <t>ORDER BY</t>
+  </si>
+  <si>
+    <t>ORDER BYで整列</t>
+  </si>
+  <si>
+    <t>データベースのインデックスの目的はどれ？</t>
+  </si>
+  <si>
+    <t>検索高速化</t>
+  </si>
+  <si>
+    <t>正規化</t>
+  </si>
+  <si>
+    <t>検索効率向上</t>
+  </si>
+  <si>
+    <t>外部キーの役割はどれ？</t>
+  </si>
+  <si>
+    <t>一意識別</t>
+  </si>
+  <si>
+    <t>表間の関連付け</t>
+  </si>
+  <si>
+    <t>高速化</t>
+  </si>
+  <si>
+    <t>主キー生成</t>
+  </si>
+  <si>
+    <t>リレーション用</t>
+  </si>
+  <si>
+    <t>トランザクションの整合性を保つための制御は？</t>
+  </si>
+  <si>
+    <t>バックアップ</t>
+  </si>
+  <si>
+    <t>排他制御</t>
+  </si>
+  <si>
+    <t>圧縮</t>
+  </si>
+  <si>
+    <t>索引</t>
+  </si>
+  <si>
+    <t>同時実行制御</t>
+  </si>
+  <si>
+    <t>情報セキュリティの可用性(Availability)とは？</t>
+  </si>
+  <si>
+    <t>漏れない</t>
+  </si>
+  <si>
+    <t>改ざん不可</t>
+  </si>
+  <si>
+    <t>使える状態</t>
+  </si>
+  <si>
+    <t>高速</t>
+  </si>
+  <si>
+    <t>使えること</t>
+  </si>
+  <si>
+    <t>ウイルス対策ソフトの主な役割は？</t>
+  </si>
+  <si>
+    <t>不正プログラム検出</t>
+  </si>
+  <si>
+    <t>マルウェア対策</t>
+  </si>
+  <si>
+    <t>ファイアウォールの目的はどれ？</t>
+  </si>
+  <si>
+    <t>通信遮断</t>
+  </si>
+  <si>
+    <t>不正通信の防止</t>
+  </si>
+  <si>
+    <t>アクセス制御</t>
+  </si>
+  <si>
+    <t>マルウェアの一種で自己増殖するものは？</t>
+  </si>
+  <si>
+    <t>トロイの木馬</t>
+  </si>
+  <si>
+    <t>ワーム</t>
+  </si>
+  <si>
+    <t>スパイウェア</t>
+  </si>
+  <si>
+    <t>ランサムウェア</t>
+  </si>
+  <si>
+    <t>ワームは自己増殖</t>
+  </si>
+  <si>
+    <t>ランサムウェアの被害として正しいものはどれ？</t>
+  </si>
+  <si>
+    <t>情報公開</t>
+  </si>
+  <si>
+    <t>PC破壊</t>
+  </si>
+  <si>
+    <t>データを人質</t>
+  </si>
+  <si>
+    <t>通信傍受</t>
+  </si>
+  <si>
+    <t>身代金要求</t>
+  </si>
+  <si>
+    <t>フローチャートで判断を表す記号は？</t>
+  </si>
+  <si>
+    <t>長方形</t>
+  </si>
+  <si>
+    <t>平行四辺形</t>
+  </si>
+  <si>
+    <t>ひし形</t>
+  </si>
+  <si>
+    <t>円</t>
+  </si>
+  <si>
+    <t>分岐はひし形</t>
+  </si>
+  <si>
+    <t>UMLのクラス図で表現されるものは？</t>
+  </si>
+  <si>
+    <t>処理手順</t>
+  </si>
+  <si>
+    <t>データ構造</t>
+  </si>
+  <si>
+    <t>通信経路</t>
+  </si>
+  <si>
+    <t>画面遷移</t>
+  </si>
+  <si>
+    <t>クラス構造</t>
+  </si>
+  <si>
+    <t>アジャイル開発の特徴はどれ？</t>
+  </si>
+  <si>
+    <t>全工程固定</t>
+  </si>
+  <si>
+    <t>短期間反復</t>
+  </si>
+  <si>
+    <t>文書重視</t>
+  </si>
+  <si>
+    <t>変更不可</t>
+  </si>
+  <si>
+    <t>反復開発</t>
+  </si>
+  <si>
+    <t>ウォーターフォール開発の特徴はどれ？</t>
+  </si>
+  <si>
+    <t>柔軟変更</t>
+  </si>
+  <si>
+    <t>後戻り前提</t>
+  </si>
+  <si>
+    <t>工程順次</t>
+  </si>
+  <si>
+    <t>短期反復</t>
+  </si>
+  <si>
+    <t>工程を順に進める</t>
+  </si>
+  <si>
+    <t>ソフトウェアテストで単体テストの目的は？</t>
+  </si>
+  <si>
+    <t>全体動作確認</t>
+  </si>
+  <si>
+    <t>モジュール単体検証</t>
+  </si>
+  <si>
+    <t>性能測定</t>
+  </si>
+  <si>
+    <t>運用確認</t>
+  </si>
+  <si>
+    <t>個別検証</t>
+  </si>
+  <si>
+    <t>プログラムで使われる変数の役割は？</t>
+  </si>
+  <si>
+    <t>処理実行</t>
+  </si>
+  <si>
+    <t>値の保存</t>
+  </si>
+  <si>
+    <t>画面表示</t>
+  </si>
+  <si>
+    <t>通信</t>
+  </si>
+  <si>
+    <t>データ保持</t>
+  </si>
+  <si>
+    <t>条件分岐に使われる制御構文はどれ？</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>switch</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>if文</t>
+  </si>
+  <si>
+    <t>繰り返し処理を行う構文はどれ？</t>
+  </si>
+  <si>
+    <t>while</t>
+  </si>
+  <si>
+    <t>try</t>
+  </si>
+  <si>
+    <t>return</t>
+  </si>
+  <si>
+    <t>while文</t>
+  </si>
+  <si>
+    <t>Webブラウザの役割はどれ？</t>
+  </si>
+  <si>
+    <t>Webページ表示</t>
+  </si>
+  <si>
+    <t>DB管理</t>
+  </si>
+  <si>
+    <t>OS管理</t>
+  </si>
+  <si>
+    <t>表示機能</t>
+  </si>
+  <si>
+    <t>URLのドメイン名の役割はどれ？</t>
+  </si>
+  <si>
+    <t>IPの代替</t>
+  </si>
+  <si>
+    <t>通信速度向上</t>
+  </si>
+  <si>
+    <t>データ圧縮</t>
+  </si>
+  <si>
+    <t>名前解決</t>
+  </si>
+  <si>
+    <t>DNSの役割はどれ？</t>
+  </si>
+  <si>
+    <t>IP変換</t>
+  </si>
+  <si>
+    <t>負荷分散</t>
+  </si>
+  <si>
+    <t>クラウドサービスのIaaSに該当するものは？</t>
+  </si>
+  <si>
+    <t>メール</t>
+  </si>
+  <si>
+    <t>仮想サーバ</t>
+  </si>
+  <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>基盤提供</t>
+  </si>
+  <si>
+    <t>SaaSの例として適切なものはどれ？</t>
+  </si>
+  <si>
+    <t>仮想マシン</t>
+  </si>
+  <si>
+    <t>ストレージ</t>
+  </si>
+  <si>
+    <t>Webメール</t>
+  </si>
+  <si>
+    <t>アプリ提供</t>
+  </si>
+  <si>
+    <t>PaaSの特徴はどれ？</t>
+  </si>
+  <si>
+    <t>インフラのみ</t>
+  </si>
+  <si>
+    <t>アプリ実行基盤</t>
+  </si>
+  <si>
+    <t>完成アプリ</t>
+  </si>
+  <si>
+    <t>端末提供</t>
+  </si>
+  <si>
+    <t>開発基盤</t>
+  </si>
+  <si>
+    <t>仮想化技術の利点はどれ？</t>
+  </si>
+  <si>
+    <t>消費電力増加</t>
+  </si>
+  <si>
+    <t>資源の有効利用</t>
+  </si>
+  <si>
+    <t>速度低下</t>
+  </si>
+  <si>
+    <t>単一用途</t>
+  </si>
+  <si>
+    <t>統合利用</t>
+  </si>
+  <si>
+    <t>IoTの特徴はどれ？</t>
+  </si>
+  <si>
+    <t>人のみ通信</t>
+  </si>
+  <si>
+    <t>モノ同士接続</t>
+  </si>
+  <si>
+    <t>高速計算専用</t>
+  </si>
+  <si>
+    <t>仮想空間</t>
+  </si>
+  <si>
+    <t>モノのインターネット</t>
+  </si>
+  <si>
+    <t>ビッグデータの特徴を表す3Vに含まれないものは？</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>Variety</t>
+  </si>
+  <si>
+    <t>Validity</t>
+  </si>
+  <si>
+    <t>3Vではない</t>
+  </si>
+  <si>
+    <t>AIで学習に用いられるデータは何と呼ばれる？</t>
+  </si>
+  <si>
+    <t>教師データ</t>
+  </si>
+  <si>
+    <t>制御データ</t>
+  </si>
+  <si>
+    <t>暗号データ</t>
+  </si>
+  <si>
+    <t>通信データ</t>
+  </si>
+  <si>
+    <t>教師あり学習</t>
+  </si>
+  <si>
+    <t>機械学習で正解ラベルを用いない学習は？</t>
+  </si>
+  <si>
+    <t>教師あり</t>
+  </si>
+  <si>
+    <t>教師なし</t>
+  </si>
+  <si>
+    <t>強化</t>
+  </si>
+  <si>
+    <t>回帰</t>
+  </si>
+  <si>
+    <t>教師なし学習</t>
+  </si>
+  <si>
+    <t>強化学習の特徴はどれ？</t>
+  </si>
+  <si>
+    <t>正解データ</t>
+  </si>
+  <si>
+    <t>報酬最大化</t>
+  </si>
+  <si>
+    <t>静的処理</t>
+  </si>
+  <si>
+    <t>回帰のみ</t>
+  </si>
+  <si>
+    <t>報酬で学習</t>
+  </si>
+  <si>
+    <t>情報リテラシーとして適切な行動はどれ？</t>
+  </si>
+  <si>
+    <t>無断転載</t>
+  </si>
+  <si>
+    <t>引用明記</t>
+  </si>
+  <si>
+    <t>パスワード共有</t>
+  </si>
+  <si>
+    <t>怪しいリンククリック</t>
+  </si>
+  <si>
+    <t>著作権尊重</t>
+  </si>
+  <si>
+    <t>著作権で保護される対象はどれ？</t>
+  </si>
+  <si>
+    <t>アイデア</t>
+  </si>
+  <si>
+    <t>表現</t>
+  </si>
+  <si>
+    <t>事実</t>
+  </si>
+  <si>
+    <t>法令</t>
+  </si>
+  <si>
+    <t>表現を保護</t>
+  </si>
+  <si>
+    <t>個人情報に該当するものはどれ？</t>
+  </si>
+  <si>
+    <t>郵便番号</t>
+  </si>
+  <si>
+    <t>氏名と住所</t>
+  </si>
+  <si>
+    <t>天気</t>
+  </si>
+  <si>
+    <t>商品価格</t>
+  </si>
+  <si>
+    <t>特定可能</t>
+  </si>
+  <si>
+    <t>システム障害対策として有効なものはどれ？</t>
+  </si>
+  <si>
+    <t>冗長化</t>
+  </si>
+  <si>
+    <t>単一化</t>
+  </si>
+  <si>
+    <t>簡略化</t>
+  </si>
+  <si>
+    <t>停止</t>
+  </si>
+  <si>
+    <t>可用性向上</t>
+  </si>
+  <si>
+    <t>RAID1の特徴はどれ？</t>
+  </si>
+  <si>
+    <t>ストライピング</t>
+  </si>
+  <si>
+    <t>ミラーリング</t>
+  </si>
+  <si>
+    <t>パリティなし</t>
+  </si>
+  <si>
+    <t>高速特化</t>
+  </si>
+  <si>
+    <t>冗長構成</t>
+  </si>
+  <si>
+    <t>RAID0の特徴はどれ？</t>
+  </si>
+  <si>
+    <t>冗長性あり</t>
+  </si>
+  <si>
+    <t>高速だが冗長なし</t>
+  </si>
+  <si>
+    <t>ミラー</t>
+  </si>
+  <si>
+    <t>速度重視</t>
+  </si>
+  <si>
+    <t>バックアップの世代管理の目的は？</t>
+  </si>
+  <si>
+    <t>復旧範囲拡大</t>
+  </si>
+  <si>
+    <t>過去復元</t>
+  </si>
+  <si>
+    <t>フルバックアップの特徴はどれ？</t>
+  </si>
+  <si>
+    <t>差分のみ</t>
+  </si>
+  <si>
+    <t>全体取得</t>
+  </si>
+  <si>
+    <t>容量最小</t>
+  </si>
+  <si>
+    <t>完全取得</t>
+  </si>
+  <si>
+    <t>差分バックアップの特徴はどれ？</t>
+  </si>
+  <si>
+    <t>常に最小</t>
+  </si>
+  <si>
+    <t>前回フルとの差分</t>
+  </si>
+  <si>
+    <t>復旧不可</t>
+  </si>
+  <si>
+    <t>暗号必須</t>
+  </si>
+  <si>
+    <t>差分取得</t>
+  </si>
+  <si>
+    <t>論理削除の特徴はどれ？</t>
+  </si>
+  <si>
+    <t>物理削除</t>
+  </si>
+  <si>
+    <t>削除フラグ</t>
+  </si>
+  <si>
+    <t>完全消去</t>
+  </si>
+  <si>
+    <t>復元不可</t>
+  </si>
+  <si>
+    <t>SQLで集計を行う関数はどれ？</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>REPLACE</t>
+  </si>
+  <si>
+    <t>CAST</t>
+  </si>
+  <si>
+    <t>JOIN</t>
+  </si>
+  <si>
+    <t>SUMは集計</t>
+  </si>
+  <si>
+    <t>GROUP BYで使われる目的はどれ？</t>
+  </si>
+  <si>
+    <t>並び替え</t>
+  </si>
+  <si>
+    <t>条件指定</t>
+  </si>
+  <si>
+    <t>集計単位指定</t>
+  </si>
+  <si>
+    <t>削除</t>
+  </si>
+  <si>
+    <t>グループ化</t>
+  </si>
+  <si>
+    <t>Webサーバの役割はどれ？</t>
+  </si>
+  <si>
+    <t>メール送信</t>
+  </si>
+  <si>
+    <t>Web要求処理</t>
+  </si>
+  <si>
+    <t>OS起動</t>
+  </si>
+  <si>
+    <t>HTTP処理</t>
+  </si>
+  <si>
+    <t>HTTPステータスコード404の意味は？</t>
+  </si>
+  <si>
+    <t>成功</t>
+  </si>
+  <si>
+    <t>権限なし</t>
+  </si>
+  <si>
+    <t>見つからない</t>
+  </si>
+  <si>
+    <t>サーバエラー</t>
+  </si>
+  <si>
+    <t>Not Found</t>
+  </si>
+  <si>
+    <t>HTTPステータスコード200の意味は？</t>
+  </si>
+  <si>
+    <t>失敗</t>
+  </si>
+  <si>
+    <t>転送</t>
+  </si>
+  <si>
+    <t>未認証</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>クッキーの用途はどれ？</t>
+  </si>
+  <si>
+    <t>通信暗号化</t>
+  </si>
+  <si>
+    <t>状態保持</t>
+  </si>
+  <si>
+    <t>セッション管理</t>
+  </si>
+  <si>
+    <t>セッション管理の目的はどれ？</t>
+  </si>
+  <si>
+    <t>ユーザ識別</t>
+  </si>
+  <si>
+    <t>状態管理</t>
+  </si>
+  <si>
+    <t>クロスサイトスクリプティング(XSS)とは？</t>
+  </si>
+  <si>
+    <t>盗聴</t>
+  </si>
+  <si>
+    <t>偽装送信</t>
+  </si>
+  <si>
+    <t>悪意スクリプト実行</t>
+  </si>
+  <si>
+    <t>XSS攻撃</t>
+  </si>
+  <si>
+    <t>SQLインジェクションの対策はどれ？</t>
+  </si>
+  <si>
+    <t>入力検証</t>
+  </si>
+  <si>
+    <t>画面分割</t>
+  </si>
+  <si>
+    <t>暗号解除</t>
+  </si>
+  <si>
+    <t>入力チェック</t>
+  </si>
+  <si>
+    <t>パスワード管理で正しいものはどれ？</t>
+  </si>
+  <si>
+    <t>使い回し</t>
+  </si>
+  <si>
+    <t>短くする</t>
+  </si>
+  <si>
+    <t>複雑で一意</t>
+  </si>
+  <si>
+    <t>公開</t>
+  </si>
+  <si>
+    <t>強固な管理</t>
+  </si>
+  <si>
+    <t>OSのユーザ権限管理の目的はどれ？</t>
+  </si>
+  <si>
+    <t>安全性向上</t>
+  </si>
+  <si>
+    <t>互換性</t>
+  </si>
+  <si>
+    <t>マルチタスクOSの特徴はどれ？</t>
+  </si>
+  <si>
+    <t>単一処理</t>
+  </si>
+  <si>
+    <t>同時実行</t>
+  </si>
+  <si>
+    <t>停止専用</t>
+  </si>
+  <si>
+    <t>省電力のみ</t>
+  </si>
+  <si>
+    <t>並行処理</t>
+  </si>
+  <si>
+    <t>リアルタイムOSの特徴はどれ？</t>
+  </si>
+  <si>
+    <t>高速必須</t>
+  </si>
+  <si>
+    <t>期限保証</t>
+  </si>
+  <si>
+    <t>大容量</t>
+  </si>
+  <si>
+    <t>汎用</t>
+  </si>
+  <si>
+    <t>応答保証</t>
+  </si>
+  <si>
+    <t>エラー訂正符号の目的はどれ？</t>
+  </si>
+  <si>
+    <t>誤り検出訂正</t>
+  </si>
+  <si>
+    <t>通信信頼性</t>
+  </si>
+  <si>
+    <t>チェックサムの役割はどれ？</t>
+  </si>
+  <si>
+    <t>誤り検出</t>
+  </si>
+  <si>
+    <t>認証</t>
+  </si>
+  <si>
+    <t>整合性確認</t>
   </si>
 </sst>
 </file>
@@ -692,7 +1760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -703,7 +1771,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -722,8 +1789,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="QuizTable" displayName="QuizTable" ref="A1:I31">
-  <autoFilter ref="A1:I31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="QuizTable" displayName="QuizTable" ref="A1:I101">
+  <autoFilter ref="A1:I101" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="question"/>
@@ -1024,11 +2091,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1274,670 +2341,2700 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A9" s="4">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="4">
-        <v>2</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A10" s="4">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10">
         <v>4</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" t="s">
         <v>76</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A11" s="4">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" t="s">
         <v>82</v>
       </c>
-      <c r="G11" s="4">
-        <v>2</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A12" s="4">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" t="s">
         <v>87</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="4">
-        <v>2</v>
-      </c>
-      <c r="H12" s="4" t="s">
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
         <v>89</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A13" s="4">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" t="s">
         <v>94</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" t="s">
         <v>95</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13">
         <v>3</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" t="s">
         <v>76</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A14" s="4">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" t="s">
         <v>99</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" t="s">
         <v>100</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" t="s">
         <v>101</v>
       </c>
-      <c r="G14" s="4">
-        <v>2</v>
-      </c>
-      <c r="H14" s="4" t="s">
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14" t="s">
         <v>102</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A15" s="4">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" t="s">
         <v>107</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" t="s">
         <v>108</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15">
         <v>3</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" t="s">
         <v>69</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A16" s="4">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" t="s">
         <v>112</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" t="s">
         <v>113</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" t="s">
         <v>114</v>
       </c>
-      <c r="G16" s="4">
-        <v>2</v>
-      </c>
-      <c r="H16" s="4" t="s">
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
         <v>35</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A17" s="4">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" t="s">
         <v>117</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" t="s">
         <v>118</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" t="s">
         <v>119</v>
       </c>
-      <c r="G17" s="4">
-        <v>2</v>
-      </c>
-      <c r="H17" s="4" t="s">
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
         <v>76</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A18" s="4">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s">
         <v>121</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" t="s">
         <v>123</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" t="s">
         <v>124</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" t="s">
         <v>125</v>
       </c>
-      <c r="G18" s="4">
-        <v>2</v>
-      </c>
-      <c r="H18" s="4" t="s">
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A19" s="4">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s">
         <v>127</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" t="s">
         <v>128</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" t="s">
         <v>129</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" t="s">
         <v>130</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" t="s">
         <v>131</v>
       </c>
-      <c r="G19" s="4">
-        <v>2</v>
-      </c>
-      <c r="H19" s="4" t="s">
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19" t="s">
         <v>89</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A20" s="4">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s">
         <v>133</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" t="s">
         <v>134</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" t="s">
         <v>135</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" t="s">
         <v>136</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" t="s">
         <v>137</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20">
         <v>3</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" t="s">
         <v>102</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A21" s="4">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s">
         <v>139</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" t="s">
         <v>140</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" t="s">
         <v>141</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" t="s">
         <v>142</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" t="s">
         <v>143</v>
       </c>
-      <c r="G21" s="4">
-        <v>2</v>
-      </c>
-      <c r="H21" s="4" t="s">
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21" t="s">
         <v>76</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A22" s="4">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s">
         <v>145</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" t="s">
         <v>146</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" t="s">
         <v>147</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" t="s">
         <v>148</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" t="s">
         <v>149</v>
       </c>
-      <c r="G22" s="4">
-        <v>2</v>
-      </c>
-      <c r="H22" s="4" t="s">
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22" t="s">
         <v>69</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A23" s="4">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s">
         <v>151</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" t="s">
         <v>152</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" t="s">
         <v>153</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" t="s">
         <v>154</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" t="s">
         <v>155</v>
       </c>
-      <c r="G23" s="4">
-        <v>2</v>
-      </c>
-      <c r="H23" s="4" t="s">
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23" t="s">
         <v>35</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I23" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A24" s="4">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" t="s">
         <v>157</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" t="s">
         <v>158</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" t="s">
         <v>159</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" t="s">
         <v>160</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" t="s">
         <v>161</v>
       </c>
-      <c r="G24" s="4">
-        <v>2</v>
-      </c>
-      <c r="H24" s="4" t="s">
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
         <v>76</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I24" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A25" s="4">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" t="s">
         <v>163</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" t="s">
         <v>164</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" t="s">
         <v>165</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" t="s">
         <v>166</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" t="s">
         <v>167</v>
       </c>
-      <c r="G25" s="4">
-        <v>2</v>
-      </c>
-      <c r="H25" s="4" t="s">
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
         <v>89</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I25" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A26" s="4">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" t="s">
         <v>169</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" t="s">
         <v>170</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" t="s">
         <v>171</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" t="s">
         <v>172</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" t="s">
         <v>173</v>
       </c>
-      <c r="G26" s="4">
-        <v>2</v>
-      </c>
-      <c r="H26" s="4" t="s">
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26" t="s">
         <v>174</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A27" s="4">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" t="s">
         <v>176</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" t="s">
         <v>177</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" t="s">
         <v>178</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" t="s">
         <v>179</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" t="s">
         <v>154</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27">
         <v>3</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" t="s">
         <v>174</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A28" s="4">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" t="s">
         <v>181</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" t="s">
         <v>182</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" t="s">
         <v>183</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" t="s">
         <v>184</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" t="s">
         <v>185</v>
       </c>
-      <c r="G28" s="4">
-        <v>2</v>
-      </c>
-      <c r="H28" s="4" t="s">
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28" t="s">
         <v>174</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I28" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A29" s="4">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" t="s">
         <v>187</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" t="s">
         <v>188</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" t="s">
         <v>189</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" t="s">
         <v>113</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" t="s">
         <v>112</v>
       </c>
-      <c r="G29" s="4">
-        <v>2</v>
-      </c>
-      <c r="H29" s="4" t="s">
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29" t="s">
         <v>35</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I29" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A30" s="4">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" t="s">
         <v>191</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" t="s">
         <v>192</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" t="s">
         <v>193</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" t="s">
         <v>194</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" t="s">
         <v>195</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30">
         <v>3</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H30" t="s">
         <v>76</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="I30" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A31" s="4">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" t="s">
         <v>197</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" t="s">
         <v>198</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" t="s">
         <v>199</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" t="s">
         <v>200</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" t="s">
         <v>201</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31">
         <v>3</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H31" t="s">
         <v>55</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="I31" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>203</v>
+      </c>
+      <c r="C32">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>15</v>
+      </c>
+      <c r="E32">
+        <v>16</v>
+      </c>
+      <c r="F32">
+        <v>17</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>205</v>
+      </c>
+      <c r="C33">
+        <v>101</v>
+      </c>
+      <c r="D33">
+        <v>110</v>
+      </c>
+      <c r="E33">
+        <v>111</v>
+      </c>
+      <c r="F33">
+        <v>1000</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+      <c r="H33" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>207</v>
+      </c>
+      <c r="C34" t="s">
+        <v>208</v>
+      </c>
+      <c r="D34" t="s">
+        <v>209</v>
+      </c>
+      <c r="E34" t="s">
+        <v>210</v>
+      </c>
+      <c r="F34" t="s">
+        <v>173</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>212</v>
+      </c>
+      <c r="C35" t="s">
+        <v>213</v>
+      </c>
+      <c r="D35" t="s">
+        <v>214</v>
+      </c>
+      <c r="E35" t="s">
+        <v>215</v>
+      </c>
+      <c r="F35" t="s">
+        <v>216</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>89</v>
+      </c>
+      <c r="I35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>218</v>
+      </c>
+      <c r="C36" t="s">
+        <v>219</v>
+      </c>
+      <c r="D36" t="s">
+        <v>220</v>
+      </c>
+      <c r="E36" t="s">
+        <v>221</v>
+      </c>
+      <c r="F36" t="s">
+        <v>222</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+      <c r="H36" t="s">
+        <v>35</v>
+      </c>
+      <c r="I36" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>224</v>
+      </c>
+      <c r="C37" t="s">
+        <v>225</v>
+      </c>
+      <c r="D37" t="s">
+        <v>226</v>
+      </c>
+      <c r="E37" t="s">
+        <v>171</v>
+      </c>
+      <c r="F37" t="s">
+        <v>173</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37" t="s">
+        <v>102</v>
+      </c>
+      <c r="I37" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>228</v>
+      </c>
+      <c r="C38" t="s">
+        <v>229</v>
+      </c>
+      <c r="D38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E38" t="s">
+        <v>231</v>
+      </c>
+      <c r="F38" t="s">
+        <v>232</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="H38" t="s">
+        <v>102</v>
+      </c>
+      <c r="I38" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>234</v>
+      </c>
+      <c r="C39" t="s">
+        <v>235</v>
+      </c>
+      <c r="D39" t="s">
+        <v>236</v>
+      </c>
+      <c r="E39" t="s">
+        <v>237</v>
+      </c>
+      <c r="F39" t="s">
+        <v>238</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39" t="s">
+        <v>102</v>
+      </c>
+      <c r="I39" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>240</v>
+      </c>
+      <c r="C40">
+        <v>16</v>
+      </c>
+      <c r="D40">
+        <v>32</v>
+      </c>
+      <c r="E40">
+        <v>64</v>
+      </c>
+      <c r="F40">
+        <v>128</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40" t="s">
+        <v>76</v>
+      </c>
+      <c r="I40" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>242</v>
+      </c>
+      <c r="C41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" t="s">
+        <v>243</v>
+      </c>
+      <c r="E41" t="s">
+        <v>244</v>
+      </c>
+      <c r="F41" t="s">
+        <v>245</v>
+      </c>
+      <c r="G41">
+        <v>3</v>
+      </c>
+      <c r="H41" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>247</v>
+      </c>
+      <c r="C42" t="s">
+        <v>248</v>
+      </c>
+      <c r="D42" t="s">
+        <v>249</v>
+      </c>
+      <c r="E42" t="s">
+        <v>250</v>
+      </c>
+      <c r="F42" t="s">
+        <v>251</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42" t="s">
+        <v>76</v>
+      </c>
+      <c r="I42" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>253</v>
+      </c>
+      <c r="C43" t="s">
+        <v>254</v>
+      </c>
+      <c r="D43" t="s">
+        <v>255</v>
+      </c>
+      <c r="E43" t="s">
+        <v>256</v>
+      </c>
+      <c r="F43" t="s">
+        <v>257</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43" t="s">
+        <v>76</v>
+      </c>
+      <c r="I43" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>259</v>
+      </c>
+      <c r="C44" t="s">
+        <v>260</v>
+      </c>
+      <c r="D44" t="s">
+        <v>261</v>
+      </c>
+      <c r="E44" t="s">
+        <v>262</v>
+      </c>
+      <c r="F44" t="s">
+        <v>263</v>
+      </c>
+      <c r="G44">
+        <v>3</v>
+      </c>
+      <c r="H44" t="s">
+        <v>76</v>
+      </c>
+      <c r="I44" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>265</v>
+      </c>
+      <c r="C45">
+        <v>21</v>
+      </c>
+      <c r="D45">
+        <v>25</v>
+      </c>
+      <c r="E45">
+        <v>80</v>
+      </c>
+      <c r="F45">
+        <v>443</v>
+      </c>
+      <c r="G45">
+        <v>3</v>
+      </c>
+      <c r="H45" t="s">
+        <v>76</v>
+      </c>
+      <c r="I45" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>267</v>
+      </c>
+      <c r="C46">
+        <v>80</v>
+      </c>
+      <c r="D46">
+        <v>110</v>
+      </c>
+      <c r="E46">
+        <v>443</v>
+      </c>
+      <c r="F46">
+        <v>8080</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46" t="s">
+        <v>76</v>
+      </c>
+      <c r="I46" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C47" t="s">
+        <v>270</v>
+      </c>
+      <c r="D47" t="s">
+        <v>271</v>
+      </c>
+      <c r="E47" t="s">
+        <v>272</v>
+      </c>
+      <c r="F47" t="s">
+        <v>273</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47" t="s">
+        <v>69</v>
+      </c>
+      <c r="I47" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>275</v>
+      </c>
+      <c r="C48" t="s">
+        <v>276</v>
+      </c>
+      <c r="D48" t="s">
+        <v>277</v>
+      </c>
+      <c r="E48" t="s">
+        <v>270</v>
+      </c>
+      <c r="F48" t="s">
+        <v>107</v>
+      </c>
+      <c r="G48">
+        <v>2</v>
+      </c>
+      <c r="H48" t="s">
+        <v>69</v>
+      </c>
+      <c r="I48" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>279</v>
+      </c>
+      <c r="C49" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" t="s">
+        <v>280</v>
+      </c>
+      <c r="E49" t="s">
+        <v>263</v>
+      </c>
+      <c r="F49" t="s">
+        <v>281</v>
+      </c>
+      <c r="G49">
+        <v>2</v>
+      </c>
+      <c r="H49" t="s">
+        <v>69</v>
+      </c>
+      <c r="I49" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>283</v>
+      </c>
+      <c r="C50" t="s">
+        <v>284</v>
+      </c>
+      <c r="D50" t="s">
+        <v>285</v>
+      </c>
+      <c r="E50" t="s">
+        <v>286</v>
+      </c>
+      <c r="F50" t="s">
+        <v>287</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
+      <c r="H50" t="s">
+        <v>69</v>
+      </c>
+      <c r="I50" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>289</v>
+      </c>
+      <c r="C51" t="s">
+        <v>290</v>
+      </c>
+      <c r="D51" t="s">
+        <v>291</v>
+      </c>
+      <c r="E51" t="s">
+        <v>292</v>
+      </c>
+      <c r="F51" t="s">
+        <v>293</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+      <c r="H51" t="s">
+        <v>69</v>
+      </c>
+      <c r="I51" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>295</v>
+      </c>
+      <c r="C52" t="s">
+        <v>296</v>
+      </c>
+      <c r="D52" t="s">
+        <v>297</v>
+      </c>
+      <c r="E52" t="s">
+        <v>298</v>
+      </c>
+      <c r="F52" t="s">
+        <v>299</v>
+      </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
+      <c r="H52" t="s">
+        <v>55</v>
+      </c>
+      <c r="I52" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>301</v>
+      </c>
+      <c r="C53" t="s">
+        <v>154</v>
+      </c>
+      <c r="D53" t="s">
+        <v>302</v>
+      </c>
+      <c r="E53" t="s">
+        <v>263</v>
+      </c>
+      <c r="F53" t="s">
+        <v>290</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="H53" t="s">
+        <v>55</v>
+      </c>
+      <c r="I53" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>304</v>
+      </c>
+      <c r="C54" t="s">
+        <v>305</v>
+      </c>
+      <c r="D54" t="s">
+        <v>306</v>
+      </c>
+      <c r="E54" t="s">
+        <v>286</v>
+      </c>
+      <c r="F54" t="s">
+        <v>263</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54" t="s">
+        <v>55</v>
+      </c>
+      <c r="I54" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>308</v>
+      </c>
+      <c r="C55" t="s">
+        <v>309</v>
+      </c>
+      <c r="D55" t="s">
+        <v>310</v>
+      </c>
+      <c r="E55" t="s">
+        <v>311</v>
+      </c>
+      <c r="F55" t="s">
+        <v>312</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55" t="s">
+        <v>55</v>
+      </c>
+      <c r="I55" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>314</v>
+      </c>
+      <c r="C56" t="s">
+        <v>315</v>
+      </c>
+      <c r="D56" t="s">
+        <v>316</v>
+      </c>
+      <c r="E56" t="s">
+        <v>317</v>
+      </c>
+      <c r="F56" t="s">
+        <v>318</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="H56" t="s">
+        <v>55</v>
+      </c>
+      <c r="I56" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>320</v>
+      </c>
+      <c r="C57" t="s">
+        <v>321</v>
+      </c>
+      <c r="D57" t="s">
+        <v>322</v>
+      </c>
+      <c r="E57" t="s">
+        <v>323</v>
+      </c>
+      <c r="F57" t="s">
+        <v>324</v>
+      </c>
+      <c r="G57">
+        <v>3</v>
+      </c>
+      <c r="H57" t="s">
+        <v>89</v>
+      </c>
+      <c r="I57" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>326</v>
+      </c>
+      <c r="C58" t="s">
+        <v>327</v>
+      </c>
+      <c r="D58" t="s">
+        <v>328</v>
+      </c>
+      <c r="E58" t="s">
+        <v>329</v>
+      </c>
+      <c r="F58" t="s">
+        <v>330</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+      <c r="H58" t="s">
+        <v>89</v>
+      </c>
+      <c r="I58" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>332</v>
+      </c>
+      <c r="C59" t="s">
+        <v>333</v>
+      </c>
+      <c r="D59" t="s">
+        <v>334</v>
+      </c>
+      <c r="E59" t="s">
+        <v>335</v>
+      </c>
+      <c r="F59" t="s">
+        <v>336</v>
+      </c>
+      <c r="G59">
+        <v>2</v>
+      </c>
+      <c r="H59" t="s">
+        <v>89</v>
+      </c>
+      <c r="I59" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>338</v>
+      </c>
+      <c r="C60" t="s">
+        <v>339</v>
+      </c>
+      <c r="D60" t="s">
+        <v>340</v>
+      </c>
+      <c r="E60" t="s">
+        <v>341</v>
+      </c>
+      <c r="F60" t="s">
+        <v>342</v>
+      </c>
+      <c r="G60">
+        <v>3</v>
+      </c>
+      <c r="H60" t="s">
+        <v>89</v>
+      </c>
+      <c r="I60" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>344</v>
+      </c>
+      <c r="C61" t="s">
+        <v>345</v>
+      </c>
+      <c r="D61" t="s">
+        <v>346</v>
+      </c>
+      <c r="E61" t="s">
+        <v>347</v>
+      </c>
+      <c r="F61" t="s">
+        <v>348</v>
+      </c>
+      <c r="G61">
+        <v>2</v>
+      </c>
+      <c r="H61" t="s">
+        <v>89</v>
+      </c>
+      <c r="I61" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>350</v>
+      </c>
+      <c r="C62" t="s">
+        <v>351</v>
+      </c>
+      <c r="D62" t="s">
+        <v>352</v>
+      </c>
+      <c r="E62" t="s">
+        <v>353</v>
+      </c>
+      <c r="F62" t="s">
+        <v>354</v>
+      </c>
+      <c r="G62">
+        <v>2</v>
+      </c>
+      <c r="H62" t="s">
+        <v>21</v>
+      </c>
+      <c r="I62" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>356</v>
+      </c>
+      <c r="C63" t="s">
+        <v>357</v>
+      </c>
+      <c r="D63" t="s">
+        <v>358</v>
+      </c>
+      <c r="E63" t="s">
+        <v>359</v>
+      </c>
+      <c r="F63" t="s">
+        <v>360</v>
+      </c>
+      <c r="G63">
+        <v>2</v>
+      </c>
+      <c r="H63" t="s">
+        <v>21</v>
+      </c>
+      <c r="I63" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>362</v>
+      </c>
+      <c r="C64" t="s">
+        <v>358</v>
+      </c>
+      <c r="D64" t="s">
+        <v>363</v>
+      </c>
+      <c r="E64" t="s">
+        <v>364</v>
+      </c>
+      <c r="F64" t="s">
+        <v>365</v>
+      </c>
+      <c r="G64">
+        <v>2</v>
+      </c>
+      <c r="H64" t="s">
+        <v>21</v>
+      </c>
+      <c r="I64" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>367</v>
+      </c>
+      <c r="C65" t="s">
+        <v>154</v>
+      </c>
+      <c r="D65" t="s">
+        <v>368</v>
+      </c>
+      <c r="E65" t="s">
+        <v>369</v>
+      </c>
+      <c r="F65" t="s">
+        <v>370</v>
+      </c>
+      <c r="G65">
+        <v>2</v>
+      </c>
+      <c r="H65" t="s">
+        <v>174</v>
+      </c>
+      <c r="I65" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>372</v>
+      </c>
+      <c r="C66" t="s">
+        <v>263</v>
+      </c>
+      <c r="D66" t="s">
+        <v>373</v>
+      </c>
+      <c r="E66" t="s">
+        <v>374</v>
+      </c>
+      <c r="F66" t="s">
+        <v>375</v>
+      </c>
+      <c r="G66">
+        <v>2</v>
+      </c>
+      <c r="H66" t="s">
+        <v>76</v>
+      </c>
+      <c r="I66" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>377</v>
+      </c>
+      <c r="C67" t="s">
+        <v>263</v>
+      </c>
+      <c r="D67" t="s">
+        <v>378</v>
+      </c>
+      <c r="E67" t="s">
+        <v>305</v>
+      </c>
+      <c r="F67" t="s">
+        <v>379</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
+      </c>
+      <c r="H67" t="s">
+        <v>76</v>
+      </c>
+      <c r="I67" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>380</v>
+      </c>
+      <c r="C68" t="s">
+        <v>381</v>
+      </c>
+      <c r="D68" t="s">
+        <v>382</v>
+      </c>
+      <c r="E68" t="s">
+        <v>69</v>
+      </c>
+      <c r="F68" t="s">
+        <v>35</v>
+      </c>
+      <c r="G68">
+        <v>2</v>
+      </c>
+      <c r="H68" t="s">
+        <v>383</v>
+      </c>
+      <c r="I68" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>385</v>
+      </c>
+      <c r="C69" t="s">
+        <v>386</v>
+      </c>
+      <c r="D69" t="s">
+        <v>387</v>
+      </c>
+      <c r="E69" t="s">
+        <v>388</v>
+      </c>
+      <c r="F69" t="s">
+        <v>35</v>
+      </c>
+      <c r="G69">
+        <v>3</v>
+      </c>
+      <c r="H69" t="s">
+        <v>383</v>
+      </c>
+      <c r="I69" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>390</v>
+      </c>
+      <c r="C70" t="s">
+        <v>391</v>
+      </c>
+      <c r="D70" t="s">
+        <v>392</v>
+      </c>
+      <c r="E70" t="s">
+        <v>393</v>
+      </c>
+      <c r="F70" t="s">
+        <v>394</v>
+      </c>
+      <c r="G70">
+        <v>2</v>
+      </c>
+      <c r="H70" t="s">
+        <v>383</v>
+      </c>
+      <c r="I70" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>396</v>
+      </c>
+      <c r="C71" t="s">
+        <v>397</v>
+      </c>
+      <c r="D71" t="s">
+        <v>398</v>
+      </c>
+      <c r="E71" t="s">
+        <v>399</v>
+      </c>
+      <c r="F71" t="s">
+        <v>400</v>
+      </c>
+      <c r="G71">
+        <v>2</v>
+      </c>
+      <c r="H71" t="s">
+        <v>383</v>
+      </c>
+      <c r="I71" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>402</v>
+      </c>
+      <c r="C72" t="s">
+        <v>403</v>
+      </c>
+      <c r="D72" t="s">
+        <v>404</v>
+      </c>
+      <c r="E72" t="s">
+        <v>405</v>
+      </c>
+      <c r="F72" t="s">
+        <v>406</v>
+      </c>
+      <c r="G72">
+        <v>2</v>
+      </c>
+      <c r="H72" t="s">
+        <v>21</v>
+      </c>
+      <c r="I72" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>408</v>
+      </c>
+      <c r="C73" t="s">
+        <v>409</v>
+      </c>
+      <c r="D73" t="s">
+        <v>410</v>
+      </c>
+      <c r="E73" t="s">
+        <v>411</v>
+      </c>
+      <c r="F73" t="s">
+        <v>412</v>
+      </c>
+      <c r="G73">
+        <v>4</v>
+      </c>
+      <c r="H73" t="s">
+        <v>21</v>
+      </c>
+      <c r="I73" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>414</v>
+      </c>
+      <c r="C74" t="s">
+        <v>415</v>
+      </c>
+      <c r="D74" t="s">
+        <v>416</v>
+      </c>
+      <c r="E74" t="s">
+        <v>417</v>
+      </c>
+      <c r="F74" t="s">
+        <v>418</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74" t="s">
+        <v>21</v>
+      </c>
+      <c r="I74" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>420</v>
+      </c>
+      <c r="C75" t="s">
+        <v>421</v>
+      </c>
+      <c r="D75" t="s">
+        <v>422</v>
+      </c>
+      <c r="E75" t="s">
+        <v>423</v>
+      </c>
+      <c r="F75" t="s">
+        <v>424</v>
+      </c>
+      <c r="G75">
+        <v>2</v>
+      </c>
+      <c r="H75" t="s">
+        <v>21</v>
+      </c>
+      <c r="I75" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>426</v>
+      </c>
+      <c r="C76" t="s">
+        <v>427</v>
+      </c>
+      <c r="D76" t="s">
+        <v>428</v>
+      </c>
+      <c r="E76" t="s">
+        <v>429</v>
+      </c>
+      <c r="F76" t="s">
+        <v>430</v>
+      </c>
+      <c r="G76">
+        <v>2</v>
+      </c>
+      <c r="H76" t="s">
+        <v>21</v>
+      </c>
+      <c r="I76" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>432</v>
+      </c>
+      <c r="C77" t="s">
+        <v>433</v>
+      </c>
+      <c r="D77" t="s">
+        <v>434</v>
+      </c>
+      <c r="E77" t="s">
+        <v>435</v>
+      </c>
+      <c r="F77" t="s">
+        <v>436</v>
+      </c>
+      <c r="G77">
+        <v>2</v>
+      </c>
+      <c r="H77" t="s">
+        <v>55</v>
+      </c>
+      <c r="I77" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>438</v>
+      </c>
+      <c r="C78" t="s">
+        <v>439</v>
+      </c>
+      <c r="D78" t="s">
+        <v>440</v>
+      </c>
+      <c r="E78" t="s">
+        <v>441</v>
+      </c>
+      <c r="F78" t="s">
+        <v>442</v>
+      </c>
+      <c r="G78">
+        <v>2</v>
+      </c>
+      <c r="H78" t="s">
+        <v>55</v>
+      </c>
+      <c r="I78" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>444</v>
+      </c>
+      <c r="C79" t="s">
+        <v>445</v>
+      </c>
+      <c r="D79" t="s">
+        <v>446</v>
+      </c>
+      <c r="E79" t="s">
+        <v>447</v>
+      </c>
+      <c r="F79" t="s">
+        <v>448</v>
+      </c>
+      <c r="G79">
+        <v>2</v>
+      </c>
+      <c r="H79" t="s">
+        <v>55</v>
+      </c>
+      <c r="I79" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>450</v>
+      </c>
+      <c r="C80" t="s">
+        <v>451</v>
+      </c>
+      <c r="D80" t="s">
+        <v>452</v>
+      </c>
+      <c r="E80" t="s">
+        <v>453</v>
+      </c>
+      <c r="F80" t="s">
+        <v>454</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80" t="s">
+        <v>35</v>
+      </c>
+      <c r="I80" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>456</v>
+      </c>
+      <c r="C81" t="s">
+        <v>457</v>
+      </c>
+      <c r="D81" t="s">
+        <v>458</v>
+      </c>
+      <c r="E81" t="s">
+        <v>459</v>
+      </c>
+      <c r="F81" t="s">
+        <v>460</v>
+      </c>
+      <c r="G81">
+        <v>2</v>
+      </c>
+      <c r="H81" t="s">
+        <v>102</v>
+      </c>
+      <c r="I81" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>462</v>
+      </c>
+      <c r="C82" t="s">
+        <v>463</v>
+      </c>
+      <c r="D82" t="s">
+        <v>464</v>
+      </c>
+      <c r="E82" t="s">
+        <v>290</v>
+      </c>
+      <c r="F82" t="s">
+        <v>465</v>
+      </c>
+      <c r="G82">
+        <v>2</v>
+      </c>
+      <c r="H82" t="s">
+        <v>102</v>
+      </c>
+      <c r="I82" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>467</v>
+      </c>
+      <c r="C83" t="s">
+        <v>112</v>
+      </c>
+      <c r="D83" t="s">
+        <v>468</v>
+      </c>
+      <c r="E83" t="s">
+        <v>286</v>
+      </c>
+      <c r="F83" t="s">
+        <v>263</v>
+      </c>
+      <c r="G83">
+        <v>2</v>
+      </c>
+      <c r="H83" t="s">
+        <v>35</v>
+      </c>
+      <c r="I83" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>470</v>
+      </c>
+      <c r="C84" t="s">
+        <v>471</v>
+      </c>
+      <c r="D84" t="s">
+        <v>472</v>
+      </c>
+      <c r="E84" t="s">
+        <v>299</v>
+      </c>
+      <c r="F84" t="s">
+        <v>473</v>
+      </c>
+      <c r="G84">
+        <v>2</v>
+      </c>
+      <c r="H84" t="s">
+        <v>35</v>
+      </c>
+      <c r="I84" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>475</v>
+      </c>
+      <c r="C85" t="s">
+        <v>476</v>
+      </c>
+      <c r="D85" t="s">
+        <v>477</v>
+      </c>
+      <c r="E85" t="s">
+        <v>478</v>
+      </c>
+      <c r="F85" t="s">
+        <v>479</v>
+      </c>
+      <c r="G85">
+        <v>2</v>
+      </c>
+      <c r="H85" t="s">
+        <v>35</v>
+      </c>
+      <c r="I85" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>481</v>
+      </c>
+      <c r="C86" t="s">
+        <v>482</v>
+      </c>
+      <c r="D86" t="s">
+        <v>483</v>
+      </c>
+      <c r="E86" t="s">
+        <v>484</v>
+      </c>
+      <c r="F86" t="s">
+        <v>485</v>
+      </c>
+      <c r="G86">
+        <v>2</v>
+      </c>
+      <c r="H86" t="s">
+        <v>69</v>
+      </c>
+      <c r="I86" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>486</v>
+      </c>
+      <c r="C87" t="s">
+        <v>487</v>
+      </c>
+      <c r="D87" t="s">
+        <v>488</v>
+      </c>
+      <c r="E87" t="s">
+        <v>489</v>
+      </c>
+      <c r="F87" t="s">
+        <v>490</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87" t="s">
+        <v>69</v>
+      </c>
+      <c r="I87" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>492</v>
+      </c>
+      <c r="C88" t="s">
+        <v>493</v>
+      </c>
+      <c r="D88" t="s">
+        <v>494</v>
+      </c>
+      <c r="E88" t="s">
+        <v>495</v>
+      </c>
+      <c r="F88" t="s">
+        <v>496</v>
+      </c>
+      <c r="G88">
+        <v>3</v>
+      </c>
+      <c r="H88" t="s">
+        <v>69</v>
+      </c>
+      <c r="I88" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>498</v>
+      </c>
+      <c r="C89" t="s">
+        <v>499</v>
+      </c>
+      <c r="D89" t="s">
+        <v>500</v>
+      </c>
+      <c r="E89" t="s">
+        <v>369</v>
+      </c>
+      <c r="F89" t="s">
+        <v>501</v>
+      </c>
+      <c r="G89">
+        <v>2</v>
+      </c>
+      <c r="H89" t="s">
+        <v>174</v>
+      </c>
+      <c r="I89" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>503</v>
+      </c>
+      <c r="C90" t="s">
+        <v>504</v>
+      </c>
+      <c r="D90" t="s">
+        <v>505</v>
+      </c>
+      <c r="E90" t="s">
+        <v>506</v>
+      </c>
+      <c r="F90" t="s">
+        <v>507</v>
+      </c>
+      <c r="G90">
+        <v>3</v>
+      </c>
+      <c r="H90" t="s">
+        <v>174</v>
+      </c>
+      <c r="I90" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>509</v>
+      </c>
+      <c r="C91" t="s">
+        <v>510</v>
+      </c>
+      <c r="D91" t="s">
+        <v>504</v>
+      </c>
+      <c r="E91" t="s">
+        <v>511</v>
+      </c>
+      <c r="F91" t="s">
+        <v>512</v>
+      </c>
+      <c r="G91">
+        <v>2</v>
+      </c>
+      <c r="H91" t="s">
+        <v>174</v>
+      </c>
+      <c r="I91" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>514</v>
+      </c>
+      <c r="C92" t="s">
+        <v>515</v>
+      </c>
+      <c r="D92" t="s">
+        <v>516</v>
+      </c>
+      <c r="E92" t="s">
+        <v>155</v>
+      </c>
+      <c r="F92" t="s">
+        <v>188</v>
+      </c>
+      <c r="G92">
+        <v>2</v>
+      </c>
+      <c r="H92" t="s">
+        <v>174</v>
+      </c>
+      <c r="I92" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>518</v>
+      </c>
+      <c r="C93" t="s">
+        <v>263</v>
+      </c>
+      <c r="D93" t="s">
+        <v>519</v>
+      </c>
+      <c r="E93" t="s">
+        <v>286</v>
+      </c>
+      <c r="F93" t="s">
+        <v>292</v>
+      </c>
+      <c r="G93">
+        <v>2</v>
+      </c>
+      <c r="H93" t="s">
+        <v>174</v>
+      </c>
+      <c r="I93" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>521</v>
+      </c>
+      <c r="C94" t="s">
+        <v>522</v>
+      </c>
+      <c r="D94" t="s">
+        <v>523</v>
+      </c>
+      <c r="E94" t="s">
+        <v>524</v>
+      </c>
+      <c r="F94" t="s">
+        <v>305</v>
+      </c>
+      <c r="G94">
+        <v>3</v>
+      </c>
+      <c r="H94" t="s">
+        <v>55</v>
+      </c>
+      <c r="I94" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>526</v>
+      </c>
+      <c r="C95" t="s">
+        <v>527</v>
+      </c>
+      <c r="D95" t="s">
+        <v>528</v>
+      </c>
+      <c r="E95" t="s">
+        <v>292</v>
+      </c>
+      <c r="F95" t="s">
+        <v>529</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+      <c r="H95" t="s">
+        <v>55</v>
+      </c>
+      <c r="I95" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>531</v>
+      </c>
+      <c r="C96" t="s">
+        <v>532</v>
+      </c>
+      <c r="D96" t="s">
+        <v>533</v>
+      </c>
+      <c r="E96" t="s">
+        <v>534</v>
+      </c>
+      <c r="F96" t="s">
+        <v>535</v>
+      </c>
+      <c r="G96">
+        <v>3</v>
+      </c>
+      <c r="H96" t="s">
+        <v>55</v>
+      </c>
+      <c r="I96" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>537</v>
+      </c>
+      <c r="C97" t="s">
+        <v>286</v>
+      </c>
+      <c r="D97" t="s">
+        <v>538</v>
+      </c>
+      <c r="E97" t="s">
+        <v>112</v>
+      </c>
+      <c r="F97" t="s">
+        <v>539</v>
+      </c>
+      <c r="G97">
+        <v>2</v>
+      </c>
+      <c r="H97" t="s">
+        <v>35</v>
+      </c>
+      <c r="I97" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>540</v>
+      </c>
+      <c r="C98" t="s">
+        <v>541</v>
+      </c>
+      <c r="D98" t="s">
+        <v>542</v>
+      </c>
+      <c r="E98" t="s">
+        <v>543</v>
+      </c>
+      <c r="F98" t="s">
+        <v>544</v>
+      </c>
+      <c r="G98">
+        <v>2</v>
+      </c>
+      <c r="H98" t="s">
+        <v>35</v>
+      </c>
+      <c r="I98" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>546</v>
+      </c>
+      <c r="C99" t="s">
+        <v>547</v>
+      </c>
+      <c r="D99" t="s">
+        <v>548</v>
+      </c>
+      <c r="E99" t="s">
+        <v>549</v>
+      </c>
+      <c r="F99" t="s">
+        <v>550</v>
+      </c>
+      <c r="G99">
+        <v>2</v>
+      </c>
+      <c r="H99" t="s">
+        <v>35</v>
+      </c>
+      <c r="I99" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>552</v>
+      </c>
+      <c r="C100" t="s">
+        <v>292</v>
+      </c>
+      <c r="D100" t="s">
+        <v>553</v>
+      </c>
+      <c r="E100" t="s">
+        <v>263</v>
+      </c>
+      <c r="F100" t="s">
+        <v>286</v>
+      </c>
+      <c r="G100">
+        <v>2</v>
+      </c>
+      <c r="H100" t="s">
+        <v>76</v>
+      </c>
+      <c r="I100" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>555</v>
+      </c>
+      <c r="C101" t="s">
+        <v>263</v>
+      </c>
+      <c r="D101" t="s">
+        <v>556</v>
+      </c>
+      <c r="E101" t="s">
+        <v>292</v>
+      </c>
+      <c r="F101" t="s">
+        <v>557</v>
+      </c>
+      <c r="G101">
+        <v>2</v>
+      </c>
+      <c r="H101" t="s">
+        <v>76</v>
+      </c>
+      <c r="I101" t="s">
+        <v>558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>